<commit_message>
<Upd><UploadFTAMaster><Upd Issue List FTA Master>
</commit_message>
<xml_diff>
--- a/PECGI_SPC/Template/Template FTA Action.xlsx
+++ b/PECGI_SPC/Template/Template FTA Action.xlsx
@@ -13,13 +13,35 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>TOS37</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Mandatory Input
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>FTAID</t>
-  </si>
-  <si>
-    <t>Action ID</t>
   </si>
   <si>
     <t>Action Name</t>
@@ -35,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +89,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -136,6 +165,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -144,9 +176,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,38 +471,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
+    <row r="1" spans="1:3" ht="15.75">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>4</v>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -482,5 +507,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>